<commit_message>
updates to the way the tests are run
</commit_message>
<xml_diff>
--- a/Automation/runs/Run.xlsx
+++ b/Automation/runs/Run.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/runs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6263" yWindow="1238" windowWidth="28823" windowHeight="14543" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4780" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="4" r:id="rId2"/>
     <sheet name="Configs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -154,10 +159,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>patient.tests.LoginTest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>baseUrl</t>
   </si>
   <si>
@@ -219,17 +220,20 @@
   <si>
     <t>chrome</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.web.tests.LoginTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -244,13 +248,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -259,7 +263,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -267,21 +271,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -289,7 +293,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -371,14 +375,14 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -728,23 +732,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="36.1328125" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,18 +768,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -787,7 +791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -798,7 +802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -809,7 +813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -820,7 +824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -831,7 +835,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -842,7 +846,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -853,7 +857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -864,7 +868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -875,7 +879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -886,34 +890,34 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
@@ -930,22 +934,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.1328125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.1328125" style="3"/>
+    <col min="3" max="3" width="12.1640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -953,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
@@ -961,15 +965,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -977,7 +981,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -985,7 +989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -993,9 +997,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="str">
         <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
@@ -1004,15 +1008,15 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -1020,7 +1024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1028,7 +1032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -1036,111 +1040,111 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
     </row>
   </sheetData>
@@ -1168,7 +1172,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Configs!$A$2:$A$10</xm:f>
           </x14:formula1>
@@ -1181,49 +1185,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>